<commit_message>
setting up file download
</commit_message>
<xml_diff>
--- a/Mishberech/MishBerech.xlsx
+++ b/Mishberech/MishBerech.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KTM\python\msutils\Mishberech\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KTM\Documents\EMK\Mishberech\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1041C9D-E7A9-417E-9085-7D1F0F3DFF2A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97E6C6AE-C79E-41A8-971C-A3B4EC500349}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9465" xr2:uid="{90422A7B-9DA7-4DD5-B2C5-D83D49DD6A73}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9465" activeTab="1" xr2:uid="{90422A7B-9DA7-4DD5-B2C5-D83D49DD6A73}"/>
   </bookViews>
   <sheets>
     <sheet name="Updates" sheetId="1" r:id="rId1"/>
@@ -806,8 +806,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9238DDAD-9B68-46FA-9D94-640A604216C3}">
   <dimension ref="B1:F37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:XFD9"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1401,24 +1401,24 @@
     <hyperlink ref="F7" r:id="rId3" display="mailto:adamossip@gmail.com" xr:uid="{9AD0D557-856C-493F-B3FB-1CB15D54E063}"/>
     <hyperlink ref="F8" r:id="rId4" display="mailto:adamossip@gmail.com" xr:uid="{CE266499-7736-423E-B7AF-82AB96714421}"/>
     <hyperlink ref="F17" r:id="rId5" display="mailto:adamossip@gmail.com" xr:uid="{F78E552A-E86A-48B5-B3EA-2E4AB2F6EAA5}"/>
-    <hyperlink ref="F28" r:id="rId6" display="mailto:robertehousman@gmail.com" xr:uid="{9649E614-D4A1-418E-980F-53E103DD538D}"/>
-    <hyperlink ref="F10" r:id="rId7" display="mailto:vrflash@gmail.com" xr:uid="{FF16932E-62BE-4B41-BC17-4D18425E0C24}"/>
-    <hyperlink ref="F15" r:id="rId8" display="mailto:anngeller@gmail.com" xr:uid="{9F61876E-9ADD-4803-A029-8C267C384860}"/>
-    <hyperlink ref="F13" r:id="rId9" display="mailto:tamarking@gmail.com" xr:uid="{07914EAE-9BE4-4258-8341-DD8CE46B3F54}"/>
-    <hyperlink ref="F14" r:id="rId10" display="mailto:tamarking@gmail.com" xr:uid="{F9B7DCE6-AA0C-40DC-880A-58C01AB8D642}"/>
-    <hyperlink ref="F16" r:id="rId11" display="mailto:agilson1234@msn.com" xr:uid="{EBD15E16-2821-4AEF-A4EE-E25FF56769F4}"/>
-    <hyperlink ref="F19" r:id="rId12" display="mailto:israel.d.gale@gmail.com" xr:uid="{DC695038-8920-4D34-B76B-1C32BA8F3C48}"/>
-    <hyperlink ref="F18" r:id="rId13" display="mailto:deansolomon@rcn.com" xr:uid="{EB70532F-EFF9-4343-9FB9-DC0DB64F7F63}"/>
-    <hyperlink ref="F23" r:id="rId14" display="mailto:deansolomon@rcn.com" xr:uid="{C6D0D8D4-1C76-4B62-9885-7F2F62BF8540}"/>
-    <hyperlink ref="F11" r:id="rId15" display="mailto:garydp@fastmail.com" xr:uid="{CF79A20F-5A21-4C97-B7BF-D92F09952777}"/>
-    <hyperlink ref="F24" r:id="rId16" display="mailto:srd2725@gmail.com" xr:uid="{B84F5A08-6F9D-446D-8ADC-7988272E3C60}"/>
-    <hyperlink ref="F25" r:id="rId17" display="mailto:jnb821@rcn.com" xr:uid="{53440A7D-DAD0-4C36-902E-4B17F6193603}"/>
-    <hyperlink ref="F26" r:id="rId18" display="mailto:mariya.nudel@gmail.com" xr:uid="{4146CAC3-0F7E-4356-BCEF-22AA2FAB9B68}"/>
-    <hyperlink ref="F27" r:id="rId19" display="mailto:mariya.nudel@gmail.com" xr:uid="{728CC745-E795-4D87-887D-3BBB955B653A}"/>
-    <hyperlink ref="F31" r:id="rId20" display="mailto:yadinoe@gmail.com" xr:uid="{D71E9E20-E3F8-457C-9EAF-E9E4FD4324CF}"/>
-    <hyperlink ref="F30" r:id="rId21" display="mailto:healingmindfully@gmail.com" xr:uid="{3148726A-4AA3-46F1-9B00-1C243A1F2E2A}"/>
-    <hyperlink ref="F29" r:id="rId22" display="mailto:sara.michael.salzberg@gmail.com" xr:uid="{D3D20756-7BFC-4BD6-A19B-D1C27D110D73}"/>
-    <hyperlink ref="F9" r:id="rId23" display="mailto:robertehousman@gmail.com" xr:uid="{62C67905-AD4E-4B7C-89BC-0D8F00BC1DF3}"/>
+    <hyperlink ref="F9" r:id="rId6" display="mailto:robertehousman@gmail.com" xr:uid="{62C67905-AD4E-4B7C-89BC-0D8F00BC1DF3}"/>
+    <hyperlink ref="F28" r:id="rId7" display="mailto:robertehousman@gmail.com" xr:uid="{9649E614-D4A1-418E-980F-53E103DD538D}"/>
+    <hyperlink ref="F10" r:id="rId8" display="mailto:vrflash@gmail.com" xr:uid="{FF16932E-62BE-4B41-BC17-4D18425E0C24}"/>
+    <hyperlink ref="F15" r:id="rId9" display="mailto:anngeller@gmail.com" xr:uid="{9F61876E-9ADD-4803-A029-8C267C384860}"/>
+    <hyperlink ref="F13" r:id="rId10" display="mailto:tamarking@gmail.com" xr:uid="{07914EAE-9BE4-4258-8341-DD8CE46B3F54}"/>
+    <hyperlink ref="F14" r:id="rId11" display="mailto:tamarking@gmail.com" xr:uid="{F9B7DCE6-AA0C-40DC-880A-58C01AB8D642}"/>
+    <hyperlink ref="F16" r:id="rId12" display="mailto:agilson1234@msn.com" xr:uid="{EBD15E16-2821-4AEF-A4EE-E25FF56769F4}"/>
+    <hyperlink ref="F19" r:id="rId13" display="mailto:israel.d.gale@gmail.com" xr:uid="{DC695038-8920-4D34-B76B-1C32BA8F3C48}"/>
+    <hyperlink ref="F18" r:id="rId14" display="mailto:deansolomon@rcn.com" xr:uid="{EB70532F-EFF9-4343-9FB9-DC0DB64F7F63}"/>
+    <hyperlink ref="F23" r:id="rId15" display="mailto:deansolomon@rcn.com" xr:uid="{C6D0D8D4-1C76-4B62-9885-7F2F62BF8540}"/>
+    <hyperlink ref="F11" r:id="rId16" display="mailto:garydp@fastmail.com" xr:uid="{CF79A20F-5A21-4C97-B7BF-D92F09952777}"/>
+    <hyperlink ref="F24" r:id="rId17" display="mailto:srd2725@gmail.com" xr:uid="{B84F5A08-6F9D-446D-8ADC-7988272E3C60}"/>
+    <hyperlink ref="F25" r:id="rId18" display="mailto:jnb821@rcn.com" xr:uid="{53440A7D-DAD0-4C36-902E-4B17F6193603}"/>
+    <hyperlink ref="F26" r:id="rId19" display="mailto:mariya.nudel@gmail.com" xr:uid="{4146CAC3-0F7E-4356-BCEF-22AA2FAB9B68}"/>
+    <hyperlink ref="F27" r:id="rId20" display="mailto:mariya.nudel@gmail.com" xr:uid="{728CC745-E795-4D87-887D-3BBB955B653A}"/>
+    <hyperlink ref="F31" r:id="rId21" display="mailto:yadinoe@gmail.com" xr:uid="{D71E9E20-E3F8-457C-9EAF-E9E4FD4324CF}"/>
+    <hyperlink ref="F30" r:id="rId22" display="mailto:healingmindfully@gmail.com" xr:uid="{3148726A-4AA3-46F1-9B00-1C243A1F2E2A}"/>
+    <hyperlink ref="F29" r:id="rId23" display="mailto:sara.michael.salzberg@gmail.com" xr:uid="{D3D20756-7BFC-4BD6-A19B-D1C27D110D73}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId24"/>
@@ -1429,8 +1429,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF342225-7833-445C-BE48-B1FD2F133D14}">
   <dimension ref="B1:E37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2051,6 +2051,5 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>